<commit_message>
new Scte_vt result changes
</commit_message>
<xml_diff>
--- a/src/test/resources/Test_datas/SCTE_VT/Book1.xlsx
+++ b/src/test/resources/Test_datas/SCTE_VT/Book1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17580" windowHeight="5205" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17580" windowHeight="5205"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -379,8 +379,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -414,7 +414,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="A1:D1"/>
     </sheetView>
   </sheetViews>

</xml_diff>